<commit_message>
- Adjusted amount of test data.
</commit_message>
<xml_diff>
--- a/Data/Form.xlsx
+++ b/Data/Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tnegherb\Documents\UiPath\BasicsOfUIAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tnegherb\Documents\UiPath\UiPath-BasicsOfUIAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036F81D0-F3D1-41F5-9970-E4C200EA9A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191D3ECC-33D6-4006-9278-43B183172AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2730" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -88,33 +88,6 @@
   </si>
   <si>
     <t>+1 555-5559</t>
-  </si>
-  <si>
-    <t>+1 555-5560</t>
-  </si>
-  <si>
-    <t>+1 555-5561</t>
-  </si>
-  <si>
-    <t>+1 555-5562</t>
-  </si>
-  <si>
-    <t>+1 555-5563</t>
-  </si>
-  <si>
-    <t>+1 555-5564</t>
-  </si>
-  <si>
-    <t>+1 555-5565</t>
-  </si>
-  <si>
-    <t>+1 555-5566</t>
-  </si>
-  <si>
-    <t>+1 555-5567</t>
-  </si>
-  <si>
-    <t>+1 555-5568</t>
   </si>
 </sst>
 </file>
@@ -439,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,213 +567,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>